<commit_message>
Update graphs and spreadsheets
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024.z.graph.xlsx
+++ b/statistics_files/2024/2024.z.graph.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\2024 files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D3E721-C098-4C52-BAD4-23D0D7CDDFEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CA2860-9C16-4E85-8EEC-2D6A2C278F87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1044,6 +1044,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>83661</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2129,12 +2132,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2154,7 +2157,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2170,8 +2173,11 @@
       <c r="E2">
         <v>89666</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>83661</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2188,7 +2194,7 @@
         <v>84022</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2205,7 +2211,7 @@
         <v>98440</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2222,7 +2228,7 @@
         <v>84778</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2239,7 +2245,7 @@
         <v>95894</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2256,7 +2262,7 @@
         <v>114493</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2273,7 +2279,7 @@
         <v>101818</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2290,7 +2296,7 @@
         <v>98924</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2307,7 +2313,7 @@
         <v>89740</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>89776</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2341,7 +2347,7 @@
         <v>84962</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2358,7 +2364,7 @@
         <v>75603</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2368,7 +2374,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2376,7 +2382,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2384,7 +2390,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2392,7 +2398,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2400,7 +2406,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2408,7 +2414,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2416,7 +2422,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2424,7 +2430,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2432,7 +2438,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2440,7 +2446,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2448,7 +2454,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2456,7 +2462,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2464,7 +2470,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2472,7 +2478,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>

</xml_diff>